<commit_message>
W08 : Build Fixed
</commit_message>
<xml_diff>
--- a/Assets/Excels/ShurikenDB.xlsx
+++ b/Assets/Excels/ShurikenDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\W07_BSHSMZOHICSM\Assets\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F961892-E421-433A-A7CE-4958C44E89AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C924AF-A2FD-4BF8-AC30-E0F9FD86DD31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13980" xr2:uid="{C7371B68-9CBA-4B53-9EC5-2D48B24F01A9}"/>
   </bookViews>
@@ -63,10 +63,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>수리검을 하나 더 가질 수 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>meritAmount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -95,10 +91,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MoveSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Cartridge</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -111,103 +103,110 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>체력 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격력 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtkDmg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대시 수 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최대 대시 수가 1 늘어납니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DashNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최대사거리 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저주</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>던지는 수리검의 수가 2개 늘어납니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돌아와!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력이 20 증가합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격력이 5 증가합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차징 단계가 1 늘어납니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수리검이 바닥에 떨어지면 자동으로 주인에게 돌아옵니다.(중첩불가)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수리검이 폭발을 일으킵니다!(중첩불가)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수리검에 유도 기능이 생깁니다.(중첩불가)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신의 체력이 50으로 고정됩니다. 수리검을 상대에게 3번 맞추면 상대가 즉사합니다.(중첩불가)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수리검을 두 개 더 가질 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수리검의 차징 속도가 100% 증가합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차징 속도 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>ChargeSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>체력 증가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>none</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격력 증가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AtkDmg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대시 수 증가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최대 대시 수가 1 늘어납니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DashNum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최대사거리 증가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>차징속도 감소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수리검의 차징 속도가 50% 감소합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>저주</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>던지는 수리검의 수가 2개 늘어납니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>돌아와!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>none</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>체력이 20 증가합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격력이 5 증가합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>차징 단계가 1 늘어납니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수리검이 벽에 부딪히면 튕깁니다. 튕긴 수리검은 2배의 데미지를 줍니다.(중첩불가)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수리검이 바닥에 떨어지면 자동으로 주인에게 돌아옵니다.(중첩불가)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수리검이 폭발을 일으킵니다!(중첩불가)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수리검에 유도 기능이 생깁니다.(중첩불가)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수리검이 거미줄을 소환합니다. 거미줄 안에 있는 적은 대시할 수 없습니다.(중첩불가)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신의 체력이 50으로 고정됩니다. 수리검을 상대에게 3번 맞추면 상대가 즉사합니다.(중첩불가)</t>
+  </si>
+  <si>
+    <t>수리검이 벽에 부딪히면 튕깁니다. 튕긴 수리검은 1.5배의 데미지를 줍니다.(중첩불가)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수리검이 거미줄을 소환합니다. 거미줄 안에서는 느려지고 대시할 수 없습니다.(중첩불가)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -586,7 +585,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -610,19 +609,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -630,22 +629,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1">
         <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -656,22 +655,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1">
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -685,22 +684,22 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -708,22 +707,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
@@ -734,22 +733,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -760,25 +759,25 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="H7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -789,19 +788,19 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1">
         <v>25</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
@@ -812,22 +811,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H9" s="1">
         <v>1</v>
@@ -841,19 +840,19 @@
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H10" s="1">
         <v>30</v>
@@ -867,19 +866,19 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="H11" s="1">
         <v>5</v>
@@ -893,19 +892,19 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H12" s="1">
         <v>10</v>
@@ -919,19 +918,19 @@
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H13" s="1">
         <v>20</v>
@@ -942,22 +941,22 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>

</xml_diff>